<commit_message>
Added the temperature dataset for growth potential modeling, still working on the Nushagak dataframe.
</commit_message>
<xml_diff>
--- a/fish/New Microsoft Excel Worksheet.xlsx
+++ b/fish/New Microsoft Excel Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npwil\OneDrive\Desktop\UAF Research Work\UAF Research Projects\Coho Growth and Temperature (Larson and Schoen)\SWSHP-Bristol-Bay-Thermal-Diversity\fish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6364DE45-ECAA-4763-AB39-A97214A07B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8BC9F8-1FF4-46A2-A0CA-0A65B4678904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="B2" sqref="B2:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>